<commit_message>
Including stats of Free Answering
</commit_message>
<xml_diff>
--- a/ExcelExport/AllAverage_Feedback.xlsx
+++ b/ExcelExport/AllAverage_Feedback.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,26 @@
           <t>Free Lies Sec.</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t># Trues</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t># Lies</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t># Free Trues</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t># Free Lies</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -475,16 +495,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.04908548616373676</v>
+        <v>-0.04762177186784809</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04255880606728162</v>
+        <v>0.04495756990159295</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1137592214223852</v>
+        <v>0.1177978128723235</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03984730884916401</v>
+        <v>0.0479405232405964</v>
       </c>
       <c r="G2" t="n">
         <v>2.7025673</v>
@@ -498,6 +518,18 @@
       <c r="J2" t="n">
         <v>3.9617291</v>
       </c>
+      <c r="L2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M2" t="n">
+        <v>10</v>
+      </c>
+      <c r="N2" t="n">
+        <v>8</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -506,16 +538,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1038554498967673</v>
+        <v>0.107481103508598</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1569394565889218</v>
+        <v>0.1617039681492539</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.03999876354134869</v>
+        <v>-0.0381621483487045</v>
       </c>
       <c r="E3" t="n">
-        <v>0.242339260329144</v>
+        <v>0.2485940006675374</v>
       </c>
       <c r="G3" t="n">
         <v>2.85374235</v>
@@ -529,6 +561,18 @@
       <c r="J3" t="n">
         <v>2.256990883333333</v>
       </c>
+      <c r="L3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -537,16 +581,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0828477790933501</v>
+        <v>0.08311790308958619</v>
       </c>
       <c r="C4" t="n">
-        <v>0.06339772054387177</v>
+        <v>0.06189214622931673</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05197607075615903</v>
+        <v>0.0511929751519607</v>
       </c>
       <c r="E4" t="n">
-        <v>0.07901899014834457</v>
+        <v>0.07789183443763835</v>
       </c>
       <c r="G4" t="n">
         <v>2.45684985</v>
@@ -560,6 +604,18 @@
       <c r="J4" t="n">
         <v>2.51434945</v>
       </c>
+      <c r="L4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -568,16 +624,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01208085642232205</v>
+        <v>0.01299609428079811</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1267892046771231</v>
+        <v>0.1275747575143158</v>
       </c>
       <c r="D5" t="n">
-        <v>0.210588095641532</v>
+        <v>0.2123092255702406</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1098086217665026</v>
+        <v>0.1087258918827383</v>
       </c>
       <c r="G5" t="n">
         <v>1.50958319</v>
@@ -591,6 +647,18 @@
       <c r="J5" t="n">
         <v>1.406710633333333</v>
       </c>
+      <c r="L5" t="n">
+        <v>10</v>
+      </c>
+      <c r="M5" t="n">
+        <v>10</v>
+      </c>
+      <c r="N5" t="n">
+        <v>7</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -599,16 +667,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2652751340675051</v>
+        <v>0.2717126667191195</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.1382934443327251</v>
+        <v>-0.1275451596305487</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2103438243326705</v>
+        <v>0.2140809321972516</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8107227821097872</v>
+        <v>0.8197452730118098</v>
       </c>
       <c r="G6" t="n">
         <v>3.19163143</v>
@@ -622,6 +690,18 @@
       <c r="J6" t="n">
         <v>3.586791433333334</v>
       </c>
+      <c r="L6" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" t="n">
+        <v>10</v>
+      </c>
+      <c r="N6" t="n">
+        <v>7</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -630,16 +710,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08876556443086778</v>
+        <v>0.09330843560988983</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06744418327421786</v>
+        <v>0.06872658849864427</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.01656330037034105</v>
+        <v>-0.01745157640583462</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.07689067375936948</v>
+        <v>-0.07159013563472139</v>
       </c>
       <c r="G7" t="n">
         <v>2.12568637</v>
@@ -653,6 +733,18 @@
       <c r="J7" t="n">
         <v>1.8522805</v>
       </c>
+      <c r="L7" t="n">
+        <v>10</v>
+      </c>
+      <c r="M7" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -661,16 +753,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.1147495815186289</v>
+        <v>-0.1113193579371374</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1439485164063181</v>
+        <v>0.144591303632018</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1593426804200586</v>
+        <v>0.1677156367630634</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1139899723423647</v>
+        <v>-0.1054721431556653</v>
       </c>
       <c r="G8" t="n">
         <v>1.79370888</v>
@@ -684,6 +776,18 @@
       <c r="J8" t="n">
         <v>6.99686465</v>
       </c>
+      <c r="L8" t="n">
+        <v>10</v>
+      </c>
+      <c r="M8" t="n">
+        <v>10</v>
+      </c>
+      <c r="N8" t="n">
+        <v>10</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -692,16 +796,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.104249853266268</v>
+        <v>-0.1019678352974485</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004105231408336902</v>
+        <v>0.007676501988482948</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05877596359395914</v>
+        <v>-0.05500193102709847</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.2527022493806412</v>
+        <v>-0.2480356728751577</v>
       </c>
       <c r="G9" t="n">
         <v>4.833613629999999</v>
@@ -715,6 +819,18 @@
       <c r="J9" t="n">
         <v>2.3608105</v>
       </c>
+      <c r="L9" t="n">
+        <v>10</v>
+      </c>
+      <c r="M9" t="n">
+        <v>10</v>
+      </c>
+      <c r="N9" t="n">
+        <v>8</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -723,16 +839,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.03818549472088704</v>
+        <v>0.04163922900789983</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1981471500664562</v>
+        <v>0.200278241297822</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1881574575271019</v>
+        <v>-0.1865226107058604</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3075374500012086</v>
+        <v>0.3053562308869803</v>
       </c>
       <c r="G10" t="n">
         <v>2.91808587</v>
@@ -746,6 +862,18 @@
       <c r="J10" t="n">
         <v>2.1692124</v>
       </c>
+      <c r="L10" t="n">
+        <v>10</v>
+      </c>
+      <c r="M10" t="n">
+        <v>10</v>
+      </c>
+      <c r="N10" t="n">
+        <v>8</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -754,16 +882,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.06427848138046996</v>
+        <v>0.06149143931986877</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01150740006527783</v>
+        <v>0.009947458025988945</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1015975474568218</v>
+        <v>-0.103795218466967</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07475992189545018</v>
+        <v>0.07483201451396219</v>
       </c>
       <c r="G11" t="n">
         <v>2.90639299</v>
@@ -777,6 +905,18 @@
       <c r="J11" t="n">
         <v>2.630323366666667</v>
       </c>
+      <c r="L11" t="n">
+        <v>10</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10</v>
+      </c>
+      <c r="N11" t="n">
+        <v>9</v>
+      </c>
+      <c r="O11" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -785,16 +925,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04085491067639097</v>
+        <v>0.04078119335830931</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1781389891903211</v>
+        <v>0.1801717197739482</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4576326679647795</v>
+        <v>0.4575852109408234</v>
       </c>
       <c r="E12" t="n">
-        <v>0.05765765031492402</v>
+        <v>0.06230324688604808</v>
       </c>
       <c r="G12" t="n">
         <v>2.21397769</v>
@@ -808,6 +948,18 @@
       <c r="J12" t="n">
         <v>3.698001133333334</v>
       </c>
+      <c r="L12" t="n">
+        <v>10</v>
+      </c>
+      <c r="M12" t="n">
+        <v>10</v>
+      </c>
+      <c r="N12" t="n">
+        <v>4</v>
+      </c>
+      <c r="O12" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -816,16 +968,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09922713172731708</v>
+        <v>0.1155053710488817</v>
       </c>
       <c r="C13" t="n">
-        <v>0.06781327243777618</v>
+        <v>0.08243110603500051</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1908613363455201</v>
+        <v>0.2019409617545528</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1834027062792443</v>
+        <v>0.1836924325818537</v>
       </c>
       <c r="G13" t="n">
         <v>3.20315665</v>
@@ -839,6 +991,18 @@
       <c r="J13" t="n">
         <v>4.58430496</v>
       </c>
+      <c r="L13" t="n">
+        <v>10</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10</v>
+      </c>
+      <c r="N13" t="n">
+        <v>7</v>
+      </c>
+      <c r="O13" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -847,16 +1011,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01518365943788945</v>
+        <v>0.0152479675680171</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.01415107340185172</v>
+        <v>-0.01308173958600202</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1789602565756062</v>
+        <v>0.1787191278060382</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1741313814077217</v>
+        <v>0.1741677061458269</v>
       </c>
       <c r="G14" t="n">
         <v>3.07635271</v>
@@ -870,6 +1034,18 @@
       <c r="J14" t="n">
         <v>7.16894535</v>
       </c>
+      <c r="L14" t="n">
+        <v>10</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10</v>
+      </c>
+      <c r="N14" t="n">
+        <v>5</v>
+      </c>
+      <c r="O14" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -878,16 +1054,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.04169149050603334</v>
+        <v>-0.04172071846149979</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0006358487039224429</v>
+        <v>0.001014223157493141</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0002465805009227023</v>
+        <v>0.0008212656316868618</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.003195330605122018</v>
+        <v>-0.004623178710214178</v>
       </c>
       <c r="G15" t="n">
         <v>7.209777990000001</v>
@@ -901,6 +1077,18 @@
       <c r="J15" t="n">
         <v>4.011589625</v>
       </c>
+      <c r="L15" t="n">
+        <v>10</v>
+      </c>
+      <c r="M15" t="n">
+        <v>10</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6</v>
+      </c>
+      <c r="O15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -909,13 +1097,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.06261729359516513</v>
+        <v>0.0629556080980055</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.006250588341392223</v>
+        <v>-0.001180259424711383</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.1095593357564544</v>
+        <v>-0.1067852262153993</v>
       </c>
       <c r="G16" t="n">
         <v>4.350084</v>
@@ -926,6 +1114,15 @@
       <c r="I16" t="n">
         <v>3.13389083</v>
       </c>
+      <c r="L16" t="n">
+        <v>10</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10</v>
+      </c>
+      <c r="N16" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -934,13 +1131,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.06309624188301607</v>
+        <v>0.06204703187343687</v>
       </c>
       <c r="C17" t="n">
-        <v>0.04590540288748059</v>
+        <v>0.04502700709106415</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.07152867342844713</v>
+        <v>-0.07255200997378244</v>
       </c>
       <c r="G17" t="n">
         <v>3.67977719</v>
@@ -950,6 +1147,15 @@
       </c>
       <c r="I17" t="n">
         <v>3.45271485</v>
+      </c>
+      <c r="L17" t="n">
+        <v>10</v>
+      </c>
+      <c r="M17" t="n">
+        <v>10</v>
+      </c>
+      <c r="N17" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected index problem with excel
</commit_message>
<xml_diff>
--- a/ExcelExport/AllAverage_Feedback.xlsx
+++ b/ExcelExport/AllAverage_Feedback.xlsx
@@ -749,7 +749,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>F29_14</t>
+          <t>F27_19</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -761,9 +761,6 @@
       <c r="D8" t="n">
         <v>0.1677156367630634</v>
       </c>
-      <c r="E8" t="n">
-        <v>-0.1054721431556653</v>
-      </c>
       <c r="G8" t="n">
         <v>1.79370888</v>
       </c>
@@ -773,9 +770,6 @@
       <c r="I8" t="n">
         <v>2.2291634</v>
       </c>
-      <c r="J8" t="n">
-        <v>6.99686465</v>
-      </c>
       <c r="L8" t="n">
         <v>10</v>
       </c>
@@ -784,15 +778,12 @@
       </c>
       <c r="N8" t="n">
         <v>10</v>
-      </c>
-      <c r="O8" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M24_18</t>
+          <t>F29_14</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -805,7 +796,7 @@
         <v>-0.05500193102709847</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.2480356728751577</v>
+        <v>-0.1054721431556653</v>
       </c>
       <c r="G9" t="n">
         <v>4.833613629999999</v>
@@ -817,7 +808,7 @@
         <v>5.5937931625</v>
       </c>
       <c r="J9" t="n">
-        <v>2.3608105</v>
+        <v>6.99686465</v>
       </c>
       <c r="L9" t="n">
         <v>10</v>
@@ -835,7 +826,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M25_5</t>
+          <t>M24_18</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -848,7 +839,7 @@
         <v>-0.1865226107058604</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3053562308869803</v>
+        <v>-0.2480356728751577</v>
       </c>
       <c r="G10" t="n">
         <v>2.91808587</v>
@@ -860,7 +851,7 @@
         <v>2.42951645</v>
       </c>
       <c r="J10" t="n">
-        <v>2.1692124</v>
+        <v>2.3608105</v>
       </c>
       <c r="L10" t="n">
         <v>10</v>
@@ -872,13 +863,13 @@
         <v>8</v>
       </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>M26_10</t>
+          <t>M25_5</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -891,7 +882,7 @@
         <v>-0.103795218466967</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07483201451396219</v>
+        <v>0.3053562308869803</v>
       </c>
       <c r="G11" t="n">
         <v>2.90639299</v>
@@ -903,7 +894,7 @@
         <v>3.102923066666667</v>
       </c>
       <c r="J11" t="n">
-        <v>2.630323366666667</v>
+        <v>2.1692124</v>
       </c>
       <c r="L11" t="n">
         <v>10</v>
@@ -915,13 +906,13 @@
         <v>9</v>
       </c>
       <c r="O11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M26_12</t>
+          <t>M26_10</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -934,7 +925,7 @@
         <v>0.4575852109408234</v>
       </c>
       <c r="E12" t="n">
-        <v>0.06230324688604808</v>
+        <v>0.07483201451396219</v>
       </c>
       <c r="G12" t="n">
         <v>2.21397769</v>
@@ -946,7 +937,7 @@
         <v>3.80306035</v>
       </c>
       <c r="J12" t="n">
-        <v>3.698001133333334</v>
+        <v>2.630323366666667</v>
       </c>
       <c r="L12" t="n">
         <v>10</v>
@@ -958,13 +949,13 @@
         <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>M26_17</t>
+          <t>M26_12</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -977,7 +968,7 @@
         <v>0.2019409617545528</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1836924325818537</v>
+        <v>0.06230324688604808</v>
       </c>
       <c r="G13" t="n">
         <v>3.20315665</v>
@@ -989,7 +980,7 @@
         <v>3.586823071428572</v>
       </c>
       <c r="J13" t="n">
-        <v>4.58430496</v>
+        <v>3.698001133333334</v>
       </c>
       <c r="L13" t="n">
         <v>10</v>
@@ -1001,13 +992,13 @@
         <v>7</v>
       </c>
       <c r="O13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>M28_7</t>
+          <t>M26_17</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1020,7 +1011,7 @@
         <v>0.1787191278060382</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1741677061458269</v>
+        <v>0.1836924325818537</v>
       </c>
       <c r="G14" t="n">
         <v>3.07635271</v>
@@ -1032,7 +1023,7 @@
         <v>4.74431044</v>
       </c>
       <c r="J14" t="n">
-        <v>7.16894535</v>
+        <v>4.58430496</v>
       </c>
       <c r="L14" t="n">
         <v>10</v>
@@ -1044,13 +1035,13 @@
         <v>5</v>
       </c>
       <c r="O14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>M31_6</t>
+          <t>M28_7</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1063,7 +1054,7 @@
         <v>0.0008212656316868618</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.004623178710214178</v>
+        <v>0.1741677061458269</v>
       </c>
       <c r="G15" t="n">
         <v>7.209777990000001</v>
@@ -1075,7 +1066,7 @@
         <v>7.13966205</v>
       </c>
       <c r="J15" t="n">
-        <v>4.011589625</v>
+        <v>7.16894535</v>
       </c>
       <c r="L15" t="n">
         <v>10</v>
@@ -1139,6 +1130,9 @@
       <c r="D17" t="n">
         <v>-0.07255200997378244</v>
       </c>
+      <c r="E17" t="n">
+        <v>-0.004623178710214178</v>
+      </c>
       <c r="G17" t="n">
         <v>3.67977719</v>
       </c>
@@ -1148,6 +1142,9 @@
       <c r="I17" t="n">
         <v>3.45271485</v>
       </c>
+      <c r="J17" t="n">
+        <v>4.011589625</v>
+      </c>
       <c r="L17" t="n">
         <v>10</v>
       </c>
@@ -1156,6 +1153,9 @@
       </c>
       <c r="N17" t="n">
         <v>6</v>
+      </c>
+      <c r="O17" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected excel data order mismatch
</commit_message>
<xml_diff>
--- a/ExcelExport/AllAverage_Feedback.xlsx
+++ b/ExcelExport/AllAverage_Feedback.xlsx
@@ -501,7 +501,7 @@
         <v>0.04495756990159295</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1177978128723235</v>
+        <v>0.1099228101172644</v>
       </c>
       <c r="E2" t="n">
         <v>0.0479405232405964</v>
@@ -547,7 +547,7 @@
         <v>-0.0381621483487045</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2485940006675374</v>
+        <v>0.2738761399158555</v>
       </c>
       <c r="G3" t="n">
         <v>2.85374235</v>
@@ -587,7 +587,7 @@
         <v>0.06189214622931673</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0511929751519607</v>
+        <v>0.1441023359669383</v>
       </c>
       <c r="E4" t="n">
         <v>0.07789183443763835</v>
@@ -630,7 +630,7 @@
         <v>0.1275747575143158</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2123092255702406</v>
+        <v>0.1869112315439355</v>
       </c>
       <c r="E5" t="n">
         <v>0.1087258918827383</v>
@@ -676,7 +676,7 @@
         <v>0.2140809321972516</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8197452730118098</v>
+        <v>0.3737553534199767</v>
       </c>
       <c r="G6" t="n">
         <v>3.19163143</v>
@@ -719,7 +719,7 @@
         <v>-0.01745157640583462</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.07159013563472139</v>
+        <v>0.1542713289716696</v>
       </c>
       <c r="G7" t="n">
         <v>2.12568637</v>
@@ -759,7 +759,7 @@
         <v>0.144591303632018</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1677156367630634</v>
+        <v>0.06868813449119934</v>
       </c>
       <c r="G8" t="n">
         <v>1.79370888</v>
@@ -793,7 +793,7 @@
         <v>0.007676501988482948</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05500193102709847</v>
+        <v>-0.03491262260628141</v>
       </c>
       <c r="E9" t="n">
         <v>-0.1054721431556653</v>
@@ -836,7 +836,7 @@
         <v>0.200278241297822</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1865226107058604</v>
+        <v>-0.0645969917924218</v>
       </c>
       <c r="E10" t="n">
         <v>-0.2480356728751577</v>
@@ -879,7 +879,7 @@
         <v>0.009947458025988945</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.103795218466967</v>
+        <v>0.07095522027031356</v>
       </c>
       <c r="E11" t="n">
         <v>0.3053562308869803</v>
@@ -922,7 +922,7 @@
         <v>0.1801717197739482</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4575852109408234</v>
+        <v>0.2325647493285459</v>
       </c>
       <c r="E12" t="n">
         <v>0.07483201451396219</v>
@@ -965,7 +965,7 @@
         <v>0.08243110603500051</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2019409617545528</v>
+        <v>0.1499872917978006</v>
       </c>
       <c r="E13" t="n">
         <v>0.06230324688604808</v>
@@ -1011,7 +1011,7 @@
         <v>0.1787191278060382</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1836924325818537</v>
+        <v>0.2597485103270794</v>
       </c>
       <c r="G14" t="n">
         <v>3.07635271</v>
@@ -1054,7 +1054,7 @@
         <v>0.0008212656316868618</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1741677061458269</v>
+        <v>0.05442711403699438</v>
       </c>
       <c r="G15" t="n">
         <v>7.209777990000001</v>
@@ -1094,7 +1094,7 @@
         <v>-0.001180259424711383</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.1067852262153993</v>
+        <v>-0.02483828526352209</v>
       </c>
       <c r="G16" t="n">
         <v>4.350084</v>
@@ -1131,7 +1131,7 @@
         <v>-0.07255200997378244</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.004623178710214178</v>
+        <v>-0.04201096303231705</v>
       </c>
       <c r="G17" t="n">
         <v>3.67977719</v>

</xml_diff>